<commit_message>
Added capability of BEMT rotor analysis
</commit_message>
<xml_diff>
--- a/sheets/BEMT.xlsx
+++ b/sheets/BEMT.xlsx
@@ -5,68 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Tutorials/pyBEMT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4AAA55-73A2-9248-960F-332BC462E664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50AF903-446A-AC48-963E-A1FACF966845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3818933C-C78F-A44D-BD0C-A20632FBDB3F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{3818933C-C78F-A44D-BD0C-A20632FBDB3F}"/>
   </bookViews>
   <sheets>
     <sheet name="BEMT" sheetId="1" r:id="rId1"/>
     <sheet name="airfoil_tables" sheetId="2" r:id="rId2"/>
     <sheet name="validation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">validation!$D$3</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">validation!$D$24:$D$69</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">validation!$E$4:$E$20</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">validation!$F$4:$F$20</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">validation!$D$3</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">validation!$C$24:$C$69</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">validation!$D$24:$D$69</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">validation!$E$4:$E$20</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">validation!$F$4:$F$20</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">validation!$C$24:$C$69</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">validation!$D$24:$D$69</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">validation!$E$4:$E$20</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">validation!$F$4:$F$20</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">validation!$C$24:$C$69</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">validation!$C$24:$C$69</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">validation!$D$24:$D$69</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">validation!$E$4:$E$20</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">validation!$F$4:$F$20</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">validation!$C$24:$C$69</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">validation!$D$24:$D$69</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">validation!$E$4:$E$20</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">validation!$F$4:$F$20</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">validation!$C$24:$C$69</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">validation!$C$4:$C$20</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">validation!$D$24:$D$69</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">validation!$E$4:$E$20</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">validation!$F$4:$F$20</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">validation!$D$24:$D$69</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">validation!$D$4:$D$20</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">validation!$E$4:$E$20</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">validation!$F$4:$F$20</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">validation!$C$24:$C$69</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -88,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -756,7 +706,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -847,27 +797,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -886,21 +815,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7903,7 +7847,7 @@
                   <c:v>0.13468643485481518</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13244612392823049</c:v>
+                  <c:v>0.13244612392822999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.130152000348078</c:v>
@@ -9225,6 +9169,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="602030496"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -28190,8 +28135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B2AB9D-DC7A-E946-B7FC-3BFE04AF1B17}">
   <dimension ref="B2:BE136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33:H33"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28230,58 +28175,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="F2" s="33" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="F2" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="J2" s="33" t="s">
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="J2" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="R2" s="33" t="s">
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="R2" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Z2" s="33" t="s">
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Z2" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AK2" s="33" t="s">
+      <c r="AA2" s="43"/>
+      <c r="AB2" s="43"/>
+      <c r="AC2" s="43"/>
+      <c r="AD2" s="43"/>
+      <c r="AE2" s="43"/>
+      <c r="AF2" s="43"/>
+      <c r="AG2" s="43"/>
+      <c r="AH2" s="43"/>
+      <c r="AI2" s="43"/>
+      <c r="AK2" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
+      <c r="AL2" s="43"/>
+      <c r="AM2" s="43"/>
+      <c r="AN2" s="43"/>
+      <c r="AO2" s="43"/>
+      <c r="AP2" s="43"/>
+      <c r="AQ2" s="43"/>
+      <c r="AR2" s="43"/>
+      <c r="AS2" s="43"/>
+      <c r="AT2" s="43"/>
       <c r="AV2" s="16" t="s">
         <v>50</v>
       </c>
@@ -28311,33 +28256,33 @@
         <v>22</v>
       </c>
       <c r="G3" s="2">
-        <f>0.5*C9</f>
+        <f>0.5*C8</f>
         <v>1.5269999999999999</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="N3" s="35" t="s">
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="N3" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="R3" s="35" t="s">
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="R3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="35" t="s">
+      <c r="V3" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="44"/>
       <c r="Z3" s="8" t="s">
         <v>33</v>
       </c>
@@ -28399,21 +28344,21 @@
         <v>42</v>
       </c>
       <c r="AV3" s="19"/>
-      <c r="AW3" s="34" t="s">
+      <c r="AW3" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="AX3" s="34"/>
-      <c r="AY3" s="34"/>
-      <c r="AZ3" s="34" t="s">
+      <c r="AX3" s="45"/>
+      <c r="AY3" s="45"/>
+      <c r="AZ3" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="BA3" s="34"/>
-      <c r="BB3" s="34"/>
-      <c r="BC3" s="34" t="s">
+      <c r="BA3" s="45"/>
+      <c r="BB3" s="45"/>
+      <c r="BC3" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="BD3" s="34"/>
-      <c r="BE3" s="36"/>
+      <c r="BD3" s="45"/>
+      <c r="BE3" s="46"/>
     </row>
     <row r="4" spans="2:57" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -28439,7 +28384,7 @@
         <v>91</v>
       </c>
       <c r="K4" s="2">
-        <f>$C$18-$C$10</f>
+        <f>$C$18-$C$9</f>
         <v>0.15000000000000002</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -28548,15 +28493,6 @@
       </c>
     </row>
     <row r="5" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F5" s="2" t="s">
         <v>31</v>
       </c>
@@ -28591,7 +28527,7 @@
         <v>30</v>
       </c>
       <c r="S5" s="2">
-        <f>($C$32+$C$5)/180*PI()</f>
+        <f>($C$32+$C$10)/180*PI()</f>
         <v>0.29670597283903599</v>
       </c>
       <c r="T5" s="2" t="s">
@@ -28602,7 +28538,7 @@
         <v>30</v>
       </c>
       <c r="W5" s="2">
-        <f>($C$33+$C$5)/180*PI()</f>
+        <f>($C$33+$C$10)/180*PI()</f>
         <v>0.29670597283903599</v>
       </c>
       <c r="X5" s="2" t="s">
@@ -28624,7 +28560,7 @@
         <v>2.8274333882308138</v>
       </c>
       <c r="AD5" s="2">
-        <f t="dataTable" ref="AD5:AD34" dt2D="0" dtr="0" r1="S4" ca="1"/>
+        <f t="dataTable" ref="AD5:AD34" dt2D="0" dtr="0" r1="S4"/>
         <v>0.13161971972094719</v>
       </c>
       <c r="AE5" s="2">
@@ -28632,7 +28568,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="AF5" s="2">
-        <f t="dataTable" ref="AF5:AF34" dt2D="0" dtr="0" r1="S4"/>
+        <f t="dataTable" ref="AF5:AF34" dt2D="0" dtr="0" r1="S4" ca="1"/>
         <v>0.96152670698992004</v>
       </c>
       <c r="AG5" s="2">
@@ -28663,7 +28599,7 @@
         <v>2.8274333882308138</v>
       </c>
       <c r="AO5" s="2">
-        <f t="dataTable" ref="AO5:AO34" dt2D="0" dtr="0" r1="W4" ca="1"/>
+        <f t="dataTable" ref="AO5:AO34" dt2D="0" dtr="0" r1="W4"/>
         <v>0.15090777810591835</v>
       </c>
       <c r="AP5" s="2">
@@ -28671,7 +28607,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="AQ5" s="2">
-        <f t="dataTable" ref="AQ5:AQ34" dt2D="0" dtr="0" r1="W4"/>
+        <f t="dataTable" ref="AQ5:AQ34" dt2D="0" dtr="0" r1="W4" ca="1"/>
         <v>0.96520909025823931</v>
       </c>
       <c r="AR5" s="2">
@@ -28718,9 +28654,11 @@
       </c>
     </row>
     <row r="6" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
+      <c r="B6" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
       <c r="F6" s="2" t="s">
         <v>114</v>
       </c>
@@ -28876,16 +28814,18 @@
       </c>
     </row>
     <row r="7" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B7" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="9">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3"/>
       <c r="F7" s="2" t="s">
         <v>105</v>
       </c>
       <c r="G7" s="30">
-        <f>$C$3/(G6*C9)</f>
+        <f>$C$3/(G6*C8)</f>
         <v>1.7860332202178961E-2</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -29004,12 +28944,14 @@
     </row>
     <row r="8" spans="2:57" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="9">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>3.0539999999999998</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="J8" s="2" t="s">
         <v>89</v>
       </c>
@@ -29030,7 +28972,7 @@
         <v>73</v>
       </c>
       <c r="S8" s="2">
-        <f xml:space="preserve"> $C$8*$C$25 / (2*PI()*$C$18)</f>
+        <f xml:space="preserve"> $C$7*$C$25 / (2*PI()*$C$18)</f>
         <v>0.16370222718023522</v>
       </c>
       <c r="T8" s="2"/>
@@ -29039,7 +28981,7 @@
         <v>73</v>
       </c>
       <c r="W8" s="2">
-        <f xml:space="preserve"> $C$8*$C$26 / (2*PI()*$C$19)</f>
+        <f xml:space="preserve"> $C$7*$C$26 / (2*PI()*$C$19)</f>
         <v>0.15915494309189535</v>
       </c>
       <c r="X8" s="2"/>
@@ -29118,19 +29060,19 @@
     </row>
     <row r="9" spans="2:57" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="9">
-        <v>3.0539999999999998</v>
+        <v>0.375</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="J9" s="2" t="s">
         <v>90</v>
       </c>
@@ -29155,7 +29097,7 @@
         <v>71</v>
       </c>
       <c r="S9" s="2">
-        <f>IF(-$C$8*($G$3-$C$18)/(2*$C$18*SIN(S4))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($G$3-$C$18)/(2*$C$18*SIN(S4)))))/PI() )</f>
+        <f>IF(-$C$7*($G$3-$C$18)/(2*$C$18*SIN(S4))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($G$3-$C$18)/(2*$C$18*SIN(S4)))))/PI() )</f>
         <v>0.99999939354124312</v>
       </c>
       <c r="T9" s="2"/>
@@ -29164,7 +29106,7 @@
         <v>71</v>
       </c>
       <c r="W9" s="2">
-        <f>IF(-$C$8*($G$3-$C$19)/(2*$C$19*SIN(W4))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($G$3-$C$19)/(2*$C$19*SIN(W4)))))/PI() )</f>
+        <f>IF(-$C$7*($G$3-$C$19)/(2*$C$19*SIN(W4))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($G$3-$C$19)/(2*$C$19*SIN(W4)))))/PI() )</f>
         <v>0.99995045915579239</v>
       </c>
       <c r="X9" s="2"/>
@@ -29243,13 +29185,13 @@
     </row>
     <row r="10" spans="2:57" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C10" s="9">
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>96</v>
@@ -29285,7 +29227,7 @@
         <v>72</v>
       </c>
       <c r="S10" s="2">
-        <f>IF(-$C$8*($C$18-$C$10)/(2*$C$18*SIN(S4))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($C$18-$C$10)/(2*$C$18*SIN(S4)))))/PI() )</f>
+        <f>IF(-$C$7*($C$18-$C$9)/(2*$C$18*SIN(S4))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($C$18-$C$9)/(2*$C$18*SIN(S4)))))/PI() )</f>
         <v>0.91989351400523434</v>
       </c>
       <c r="T10" s="2"/>
@@ -29294,7 +29236,7 @@
         <v>72</v>
       </c>
       <c r="W10" s="2">
-        <f>IF(-$C$8*($C$19-$C$10)/(2*$C$19*SIN(W4))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($C$19-$C$10)/(2*$C$19*SIN(W4)))))/PI() )</f>
+        <f>IF(-$C$7*($C$19-$C$9)/(2*$C$19*SIN(W4))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($C$19-$C$9)/(2*$C$19*SIN(W4)))))/PI() )</f>
         <v>0.977240066943313</v>
       </c>
       <c r="X10" s="2"/>
@@ -29372,7 +29314,7 @@
       </c>
     </row>
     <row r="11" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="47" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -29481,7 +29423,7 @@
       </c>
     </row>
     <row r="12" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B12" s="32"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="9" t="s">
         <v>16</v>
       </c>
@@ -29496,16 +29438,16 @@
       <c r="H12" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="J12" s="35" t="s">
+      <c r="J12" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="N12" s="35" t="s">
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="N12" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
+      <c r="O12" s="44"/>
+      <c r="P12" s="44"/>
       <c r="R12" s="2" t="s">
         <v>48</v>
       </c>
@@ -29597,7 +29539,7 @@
       </c>
     </row>
     <row r="13" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B13" s="32"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="9" t="s">
         <v>16</v>
       </c>
@@ -29713,16 +29655,16 @@
       </c>
     </row>
     <row r="14" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B14" s="32"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
       <c r="J14" s="2" t="s">
         <v>86</v>
       </c>
@@ -29834,7 +29776,7 @@
       </c>
     </row>
     <row r="15" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B15" s="32"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
@@ -29843,7 +29785,7 @@
         <v>100</v>
       </c>
       <c r="G15" s="2">
-        <f>SQRT(G10^3/(2*C41*PI()*(C9/2)^2))/1000</f>
+        <f>SQRT(G10^3/(2*C41*PI()*(C8/2)^2))/1000</f>
         <v>82.927947944833036</v>
       </c>
       <c r="H15" s="3" t="s">
@@ -29960,7 +29902,7 @@
       </c>
     </row>
     <row r="16" spans="2:57" x14ac:dyDescent="0.2">
-      <c r="B16" s="32"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="9" t="s">
         <v>16</v>
       </c>
@@ -30084,7 +30026,7 @@
       </c>
     </row>
     <row r="17" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B17" s="32"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
@@ -30093,7 +30035,7 @@
         <v>66</v>
       </c>
       <c r="G17" s="2">
-        <f>G10/($C$41*G6^2*C9^4)</f>
+        <f>G10/($C$41*G6^2*C8^4)</f>
         <v>0.13900706290509893</v>
       </c>
       <c r="H17" s="2"/>
@@ -30204,7 +30146,7 @@
       </c>
     </row>
     <row r="18" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="9">
@@ -30217,7 +30159,7 @@
         <v>67</v>
       </c>
       <c r="G18" s="2">
-        <f>G11/($C$41*G6^2*C9^5)</f>
+        <f>G11/($C$41*G6^2*C8^5)</f>
         <v>8.6075281278111364E-3</v>
       </c>
       <c r="H18" s="3"/>
@@ -30332,7 +30274,7 @@
       </c>
     </row>
     <row r="19" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B19" s="32"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="9">
         <v>0.67500000000000004</v>
       </c>
@@ -30458,7 +30400,7 @@
       </c>
     </row>
     <row r="20" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B20" s="32"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="9">
         <v>0.82499999999999996</v>
       </c>
@@ -30564,7 +30506,7 @@
       </c>
     </row>
     <row r="21" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B21" s="32"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="9">
         <v>0.97499999999999998</v>
       </c>
@@ -30572,16 +30514,16 @@
         <v>10</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="J21" s="35" t="s">
+      <c r="J21" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="N21" s="35" t="s">
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="N21" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
@@ -30663,18 +30605,18 @@
       </c>
     </row>
     <row r="22" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B22" s="32"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="9">
         <v>1.125</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
       <c r="J22" s="2" t="s">
         <v>91</v>
       </c>
@@ -30695,17 +30637,17 @@
       <c r="P22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R22" s="35" t="s">
+      <c r="R22" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
+      <c r="S22" s="44"/>
+      <c r="T22" s="44"/>
       <c r="U22" s="2"/>
-      <c r="V22" s="35" t="s">
+      <c r="V22" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
+      <c r="W22" s="44"/>
+      <c r="X22" s="44"/>
       <c r="Z22" s="2">
         <v>18</v>
       </c>
@@ -30780,21 +30722,21 @@
       </c>
     </row>
     <row r="23" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B23" s="32"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="9">
         <v>1.2749999999999999</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F23" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="47">
         <f>S20</f>
         <v>-5.785007573672063E-9</v>
       </c>
-      <c r="H23" s="32"/>
+      <c r="H23" s="47"/>
       <c r="J23" s="2" t="s">
         <v>86</v>
       </c>
@@ -30910,19 +30852,19 @@
       </c>
     </row>
     <row r="24" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B24" s="32"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="9">
         <v>1.425</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="32">
+      <c r="F24" s="45"/>
+      <c r="G24" s="47">
         <f>W20</f>
         <v>-2.4493098400163449E-9</v>
       </c>
-      <c r="H24" s="32"/>
+      <c r="H24" s="47"/>
       <c r="J24" s="2" t="s">
         <v>87</v>
       </c>
@@ -30947,7 +30889,7 @@
         <v>30</v>
       </c>
       <c r="S24" s="2">
-        <f>($C$34+$C$5)/180*PI()</f>
+        <f>($C$34+$C$10)/180*PI()</f>
         <v>0.29670597283903599</v>
       </c>
       <c r="T24" s="2" t="s">
@@ -30958,7 +30900,7 @@
         <v>30</v>
       </c>
       <c r="W24" s="2">
-        <f>($C$35+$C$5)/180*PI()</f>
+        <f>($C$35+$C$10)/180*PI()</f>
         <v>0.29670597283903599</v>
       </c>
       <c r="X24" s="2" t="s">
@@ -31038,7 +30980,7 @@
       </c>
     </row>
     <row r="25" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="47" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="9">
@@ -31047,12 +30989,12 @@
       <c r="D25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="32">
+      <c r="F25" s="45"/>
+      <c r="G25" s="47">
         <f>S39</f>
         <v>-7.1855308803742135E-9</v>
       </c>
-      <c r="H25" s="32"/>
+      <c r="H25" s="47"/>
       <c r="J25" s="2" t="s">
         <v>88</v>
       </c>
@@ -31168,19 +31110,19 @@
       </c>
     </row>
     <row r="26" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B26" s="32"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="9">
         <v>0.22500000000000001</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="32">
+      <c r="F26" s="45"/>
+      <c r="G26" s="47">
         <f>W39</f>
         <v>-5.7714195835639748E-9</v>
       </c>
-      <c r="H26" s="32"/>
+      <c r="H26" s="47"/>
       <c r="J26" s="2" t="s">
         <v>89</v>
       </c>
@@ -31292,19 +31234,19 @@
       </c>
     </row>
     <row r="27" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B27" s="32"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="9">
         <v>0.22500000000000001</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="32">
+      <c r="F27" s="45"/>
+      <c r="G27" s="47">
         <f>S58</f>
         <v>2.8131671818421022E-9</v>
       </c>
-      <c r="H27" s="32"/>
+      <c r="H27" s="47"/>
       <c r="J27" s="2" t="s">
         <v>90</v>
       </c>
@@ -31329,7 +31271,7 @@
         <v>73</v>
       </c>
       <c r="S27" s="2">
-        <f xml:space="preserve"> $C$8*$C$27 / (2*PI()*$C$20)</f>
+        <f xml:space="preserve"> $C$7*$C$27 / (2*PI()*$C$20)</f>
         <v>0.13021768071155074</v>
       </c>
       <c r="T27" s="2"/>
@@ -31338,7 +31280,7 @@
         <v>73</v>
       </c>
       <c r="W27" s="2">
-        <f xml:space="preserve"> $C$8*$C$28 / (2*PI()*$C$21)</f>
+        <f xml:space="preserve"> $C$7*$C$28 / (2*PI()*$C$21)</f>
         <v>0.10283857861322468</v>
       </c>
       <c r="X27" s="2"/>
@@ -31416,19 +31358,19 @@
       </c>
     </row>
     <row r="28" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B28" s="32"/>
+      <c r="B28" s="47"/>
       <c r="C28" s="9">
         <v>0.21</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="32">
+      <c r="F28" s="45"/>
+      <c r="G28" s="47">
         <f>W58</f>
         <v>8.1482677983385488E-10</v>
       </c>
-      <c r="H28" s="32"/>
+      <c r="H28" s="47"/>
       <c r="J28" s="2" t="s">
         <v>94</v>
       </c>
@@ -31453,7 +31395,7 @@
         <v>71</v>
       </c>
       <c r="S28" s="2">
-        <f>IF(-$C$8*($G$3-$C$20)/(2*$C$20*SIN(S23))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($G$3-$C$20)/(2*$C$20*SIN(S23)))))/PI() )</f>
+        <f>IF(-$C$7*($G$3-$C$20)/(2*$C$20*SIN(S23))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($G$3-$C$20)/(2*$C$20*SIN(S23)))))/PI() )</f>
         <v>0.99931571126568908</v>
       </c>
       <c r="T28" s="2"/>
@@ -31462,7 +31404,7 @@
         <v>71</v>
       </c>
       <c r="W28" s="2">
-        <f>IF(-$C$8*($G$3-$C$21)/(2*$C$21*SIN(W23))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($G$3-$C$21)/(2*$C$21*SIN(W23)))))/PI() )</f>
+        <f>IF(-$C$7*($G$3-$C$21)/(2*$C$21*SIN(W23))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($G$3-$C$21)/(2*$C$21*SIN(W23)))))/PI() )</f>
         <v>0.99537176520309123</v>
       </c>
       <c r="X28" s="2"/>
@@ -31540,24 +31482,24 @@
       </c>
     </row>
     <row r="29" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B29" s="32"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="9">
         <v>0.1875</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="32">
+      <c r="F29" s="45"/>
+      <c r="G29" s="47">
         <f>S77</f>
         <v>-4.7047981378833814E-9</v>
       </c>
-      <c r="H29" s="32"/>
+      <c r="H29" s="47"/>
       <c r="R29" s="2" t="s">
         <v>72</v>
       </c>
       <c r="S29" s="2">
-        <f>IF(-$C$8*($C$20-$C$10)/(2*$C$20*SIN(S23))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($C$20-$C$10)/(2*$C$20*SIN(S23)))))/PI() )</f>
+        <f>IF(-$C$7*($C$20-$C$9)/(2*$C$20*SIN(S23))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($C$20-$C$9)/(2*$C$20*SIN(S23)))))/PI() )</f>
         <v>0.99203993604646279</v>
       </c>
       <c r="T29" s="2"/>
@@ -31566,7 +31508,7 @@
         <v>72</v>
       </c>
       <c r="W29" s="2">
-        <f>IF(-$C$8*($C$21-$C$10)/(2*$C$21*SIN(W23))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($C$21-$C$10)/(2*$C$21*SIN(W23)))))/PI() )</f>
+        <f>IF(-$C$7*($C$21-$C$9)/(2*$C$21*SIN(W23))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($C$21-$C$9)/(2*$C$21*SIN(W23)))))/PI() )</f>
         <v>0.99698380515021612</v>
       </c>
       <c r="X29" s="2"/>
@@ -31644,7 +31586,7 @@
       </c>
     </row>
     <row r="30" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B30" s="32"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="9">
         <v>0.14249999999999999</v>
       </c>
@@ -31654,16 +31596,16 @@
       <c r="F30" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="G30" s="32" t="b">
+      <c r="G30" s="47" t="b">
         <f>IF(G23&lt;0.00001,IF(G24&lt;0.00001,IF(G25&lt;0.00001,IF(G26&lt;0.00001,IF(G27&lt;0.00001,IF(G28&lt;0.00001,IF(G29&lt;0.00001,TRUE,FALSE),FALSE),FALSE),FALSE),FALSE),FALSE),FALSE)</f>
         <v>1</v>
       </c>
-      <c r="H30" s="32"/>
-      <c r="J30" s="35" t="s">
+      <c r="H30" s="47"/>
+      <c r="J30" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
       <c r="R30" s="2" t="s">
         <v>70</v>
       </c>
@@ -31755,7 +31697,7 @@
       </c>
     </row>
     <row r="31" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B31" s="32"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="9">
         <v>0.12</v>
       </c>
@@ -31863,7 +31805,7 @@
       </c>
     </row>
     <row r="32" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="47" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="9">
@@ -31973,7 +31915,7 @@
       </c>
     </row>
     <row r="33" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B33" s="32"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="9">
         <v>17</v>
       </c>
@@ -32080,7 +32022,7 @@
       </c>
     </row>
     <row r="34" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B34" s="32"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="9">
         <v>17</v>
       </c>
@@ -32187,7 +32129,7 @@
       </c>
     </row>
     <row r="35" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B35" s="32"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="9">
         <v>17</v>
       </c>
@@ -32230,7 +32172,7 @@
       <c r="AI35" s="2"/>
     </row>
     <row r="36" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B36" s="32"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="9">
         <v>17</v>
       </c>
@@ -32263,33 +32205,33 @@
         <v>32.417433011526782</v>
       </c>
       <c r="X36" s="2"/>
-      <c r="Z36" s="33" t="s">
+      <c r="Z36" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="AA36" s="33"/>
-      <c r="AB36" s="33"/>
-      <c r="AC36" s="33"/>
-      <c r="AD36" s="33"/>
-      <c r="AE36" s="33"/>
-      <c r="AF36" s="33"/>
-      <c r="AG36" s="33"/>
-      <c r="AH36" s="33"/>
-      <c r="AI36" s="33"/>
-      <c r="AK36" s="33" t="s">
+      <c r="AA36" s="43"/>
+      <c r="AB36" s="43"/>
+      <c r="AC36" s="43"/>
+      <c r="AD36" s="43"/>
+      <c r="AE36" s="43"/>
+      <c r="AF36" s="43"/>
+      <c r="AG36" s="43"/>
+      <c r="AH36" s="43"/>
+      <c r="AI36" s="43"/>
+      <c r="AK36" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="AL36" s="33"/>
-      <c r="AM36" s="33"/>
-      <c r="AN36" s="33"/>
-      <c r="AO36" s="33"/>
-      <c r="AP36" s="33"/>
-      <c r="AQ36" s="33"/>
-      <c r="AR36" s="33"/>
-      <c r="AS36" s="33"/>
-      <c r="AT36" s="33"/>
+      <c r="AL36" s="43"/>
+      <c r="AM36" s="43"/>
+      <c r="AN36" s="43"/>
+      <c r="AO36" s="43"/>
+      <c r="AP36" s="43"/>
+      <c r="AQ36" s="43"/>
+      <c r="AR36" s="43"/>
+      <c r="AS36" s="43"/>
+      <c r="AT36" s="43"/>
     </row>
     <row r="37" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B37" s="32"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="9">
         <v>17</v>
       </c>
@@ -32384,7 +32326,7 @@
       </c>
     </row>
     <row r="38" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B38" s="32"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="9">
         <v>17</v>
       </c>
@@ -32486,7 +32428,7 @@
         <v>2.8274333882308138</v>
       </c>
       <c r="AD39" s="2">
-        <f t="dataTable" ref="AD39:AD68" dt2D="0" dtr="0" r1="S23" ca="1"/>
+        <f t="dataTable" ref="AD39:AD68" dt2D="0" dtr="0" r1="S23"/>
         <v>0.18263494917145773</v>
       </c>
       <c r="AE39" s="2">
@@ -32494,7 +32436,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="AF39" s="2">
-        <f t="dataTable" ref="AF39:AF68" dt2D="0" dtr="0" r1="S23"/>
+        <f t="dataTable" ref="AF39:AF68" dt2D="0" dtr="0" r1="S23" ca="1"/>
         <v>0.96914364094302141</v>
       </c>
       <c r="AG39" s="2">
@@ -32525,7 +32467,7 @@
         <v>2.8274333882308138</v>
       </c>
       <c r="AO39" s="2">
-        <f t="dataTable" ref="AO39:AO68" dt2D="0" dtr="0" r1="W23" ca="1"/>
+        <f t="dataTable" ref="AO39:AO68" dt2D="0" dtr="0" r1="W23"/>
         <v>0.20783581121173944</v>
       </c>
       <c r="AP39" s="2">
@@ -32533,7 +32475,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="AQ39" s="2">
-        <f t="dataTable" ref="AQ39:AQ68" dt2D="0" dtr="0" r1="W23"/>
+        <f t="dataTable" ref="AQ39:AQ68" dt2D="0" dtr="0" r1="W23" ca="1"/>
         <v>0.97190949455447628</v>
       </c>
       <c r="AR39" s="2">
@@ -32550,11 +32492,11 @@
       </c>
     </row>
     <row r="40" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
       <c r="Z40" s="2">
         <v>2</v>
       </c>
@@ -32638,17 +32580,17 @@
       <c r="D41" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R41" s="35" t="s">
+      <c r="R41" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="S41" s="35"/>
-      <c r="T41" s="35"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
       <c r="U41" s="2"/>
-      <c r="V41" s="35" t="s">
+      <c r="V41" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="W41" s="35"/>
-      <c r="X41" s="35"/>
+      <c r="W41" s="44"/>
+      <c r="X41" s="44"/>
       <c r="Z41" s="2">
         <v>3</v>
       </c>
@@ -32834,7 +32776,7 @@
         <v>30</v>
       </c>
       <c r="S43" s="2">
-        <f>($C$36+$C$5)/180*PI()</f>
+        <f>($C$36+$C$10)/180*PI()</f>
         <v>0.29670597283903599</v>
       </c>
       <c r="T43" s="2" t="s">
@@ -32845,7 +32787,7 @@
         <v>30</v>
       </c>
       <c r="W43" s="2">
-        <f>($C$37+$C$5)/180*PI()</f>
+        <f>($C$37+$C$10)/180*PI()</f>
         <v>0.29670597283903599</v>
       </c>
       <c r="X43" s="2" t="s">
@@ -33119,7 +33061,7 @@
         <v>73</v>
       </c>
       <c r="S46" s="2">
-        <f xml:space="preserve"> $C$8*$C$29 / (2*PI()*$C$22)</f>
+        <f xml:space="preserve"> $C$7*$C$29 / (2*PI()*$C$22)</f>
         <v>7.9577471545947673E-2</v>
       </c>
       <c r="T46" s="2"/>
@@ -33128,7 +33070,7 @@
         <v>73</v>
       </c>
       <c r="W46" s="2">
-        <f xml:space="preserve"> $C$8*$C$30 / (2*PI()*$C$23)</f>
+        <f xml:space="preserve"> $C$7*$C$30 / (2*PI()*$C$23)</f>
         <v>5.3363716213164915E-2</v>
       </c>
       <c r="X46" s="2"/>
@@ -33210,7 +33152,7 @@
         <v>71</v>
       </c>
       <c r="S47" s="2">
-        <f>IF(-$C$8*($G$3-$C$22)/(2*$C$22*SIN(S42))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($G$3-$C$22)/(2*$C$22*SIN(S42)))))/PI() )</f>
+        <f>IF(-$C$7*($G$3-$C$22)/(2*$C$22*SIN(S42))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($G$3-$C$22)/(2*$C$22*SIN(S42)))))/PI() )</f>
         <v>0.97835518326401305</v>
       </c>
       <c r="T47" s="2"/>
@@ -33219,7 +33161,7 @@
         <v>71</v>
       </c>
       <c r="W47" s="2">
-        <f>IF(-$C$8*($G$3-$C$23)/(2*$C$23*SIN(W42))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($G$3-$C$23)/(2*$C$23*SIN(W42)))))/PI() )</f>
+        <f>IF(-$C$7*($G$3-$C$23)/(2*$C$23*SIN(W42))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($G$3-$C$23)/(2*$C$23*SIN(W42)))))/PI() )</f>
         <v>0.92337472227762463</v>
       </c>
       <c r="X47" s="2"/>
@@ -33304,7 +33246,7 @@
         <v>72</v>
       </c>
       <c r="S48" s="2">
-        <f>IF(-$C$8*($C$22-$C$10)/(2*$C$22*SIN(S42))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($C$22-$C$10)/(2*$C$22*SIN(S42)))))/PI() )</f>
+        <f>IF(-$C$7*($C$22-$C$9)/(2*$C$22*SIN(S42))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($C$22-$C$9)/(2*$C$22*SIN(S42)))))/PI() )</f>
         <v>0.99884139193582311</v>
       </c>
       <c r="T48" s="2"/>
@@ -33313,7 +33255,7 @@
         <v>72</v>
       </c>
       <c r="W48" s="2">
-        <f>IF(-$C$8*($C$23-$C$10)/(2*$C$23*SIN(W42))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($C$23-$C$10)/(2*$C$23*SIN(W42)))))/PI() )</f>
+        <f>IF(-$C$7*($C$23-$C$9)/(2*$C$23*SIN(W42))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($C$23-$C$9)/(2*$C$23*SIN(W42)))))/PI() )</f>
         <v>0.99967177178655009</v>
       </c>
       <c r="X48" s="2"/>
@@ -34418,11 +34360,11 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="3"/>
-      <c r="R60" s="35" t="s">
+      <c r="R60" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="S60" s="35"/>
-      <c r="T60" s="35"/>
+      <c r="S60" s="44"/>
+      <c r="T60" s="44"/>
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
       <c r="W60" s="2"/>
@@ -34597,7 +34539,7 @@
         <v>30</v>
       </c>
       <c r="S62" s="2">
-        <f>($C$38+$C$5)/180*PI()</f>
+        <f>($C$38+$C$10)/180*PI()</f>
         <v>0.29670597283903599</v>
       </c>
       <c r="T62" s="2" t="s">
@@ -34864,7 +34806,7 @@
         <v>73</v>
       </c>
       <c r="S65" s="2">
-        <f xml:space="preserve"> $C$8*$C$31 / (2*PI()*$C$24)</f>
+        <f xml:space="preserve"> $C$7*$C$31 / (2*PI()*$C$24)</f>
         <v>4.0207564570584081E-2</v>
       </c>
       <c r="T65" s="2"/>
@@ -34950,7 +34892,7 @@
         <v>71</v>
       </c>
       <c r="S66" s="2">
-        <f>IF(-$C$8*($G$3-$C$24)/(2*$C$24*SIN(S61))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($G$3-$C$24)/(2*$C$24*SIN(S61)))))/PI() )</f>
+        <f>IF(-$C$7*($G$3-$C$24)/(2*$C$24*SIN(S61))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($G$3-$C$24)/(2*$C$24*SIN(S61)))))/PI() )</f>
         <v>0.69288800068466716</v>
       </c>
       <c r="T66" s="2"/>
@@ -35036,7 +34978,7 @@
         <v>72</v>
       </c>
       <c r="S67" s="2">
-        <f>IF(-$C$8*($C$24-$C$10)/(2*$C$24*SIN(S61))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$8*($C$24-$C$10)/(2*$C$24*SIN(S61)))))/PI() )</f>
+        <f>IF(-$C$7*($C$24-$C$9)/(2*$C$24*SIN(S61))&gt;500, 1, 2*ACOS(MIN(1, EXP(-$C$7*($C$24-$C$9)/(2*$C$24*SIN(S61)))))/PI() )</f>
         <v>0.99976548745651161</v>
       </c>
       <c r="T67" s="2"/>
@@ -35230,30 +35172,30 @@
       <c r="V70" s="2"/>
       <c r="W70" s="2"/>
       <c r="X70" s="3"/>
-      <c r="Z70" s="33" t="s">
+      <c r="Z70" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="AA70" s="33"/>
-      <c r="AB70" s="33"/>
-      <c r="AC70" s="33"/>
-      <c r="AD70" s="33"/>
-      <c r="AE70" s="33"/>
-      <c r="AF70" s="33"/>
-      <c r="AG70" s="33"/>
-      <c r="AH70" s="33"/>
-      <c r="AI70" s="33"/>
-      <c r="AK70" s="33" t="s">
+      <c r="AA70" s="43"/>
+      <c r="AB70" s="43"/>
+      <c r="AC70" s="43"/>
+      <c r="AD70" s="43"/>
+      <c r="AE70" s="43"/>
+      <c r="AF70" s="43"/>
+      <c r="AG70" s="43"/>
+      <c r="AH70" s="43"/>
+      <c r="AI70" s="43"/>
+      <c r="AK70" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="AL70" s="33"/>
-      <c r="AM70" s="33"/>
-      <c r="AN70" s="33"/>
-      <c r="AO70" s="33"/>
-      <c r="AP70" s="33"/>
-      <c r="AQ70" s="33"/>
-      <c r="AR70" s="33"/>
-      <c r="AS70" s="33"/>
-      <c r="AT70" s="33"/>
+      <c r="AL70" s="43"/>
+      <c r="AM70" s="43"/>
+      <c r="AN70" s="43"/>
+      <c r="AO70" s="43"/>
+      <c r="AP70" s="43"/>
+      <c r="AQ70" s="43"/>
+      <c r="AR70" s="43"/>
+      <c r="AS70" s="43"/>
+      <c r="AT70" s="43"/>
     </row>
     <row r="71" spans="4:46" x14ac:dyDescent="0.2">
       <c r="R71" s="2" t="s">
@@ -35414,7 +35356,7 @@
         <v>2.8274333882308138</v>
       </c>
       <c r="AD73" s="2">
-        <f t="dataTable" ref="AD73:AD102" dt2D="0" dtr="0" r1="S42" ca="1"/>
+        <f t="dataTable" ref="AD73:AD102" dt2D="0" dtr="0" r1="S42"/>
         <v>0.2252761116937701</v>
       </c>
       <c r="AE73" s="2">
@@ -35422,7 +35364,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="AF73" s="2">
-        <f t="dataTable" ref="AF73:AF102" dt2D="0" dtr="0" r1="S42"/>
+        <f t="dataTable" ref="AF73:AF102" dt2D="0" dtr="0" r1="S42" ca="1"/>
         <v>0.97371053655894602</v>
       </c>
       <c r="AG73" s="2">
@@ -35453,7 +35395,7 @@
         <v>2.8274333882308138</v>
       </c>
       <c r="AO73" s="2">
-        <f t="dataTable" ref="AO73:AO102" dt2D="0" dtr="0" r1="W42" ca="1"/>
+        <f t="dataTable" ref="AO73:AO102" dt2D="0" dtr="0" r1="W42"/>
         <v>0.24354650109782877</v>
       </c>
       <c r="AP73" s="2">
@@ -35461,7 +35403,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="AQ73" s="2">
-        <f t="dataTable" ref="AQ73:AQ102" dt2D="0" dtr="0" r1="W42"/>
+        <f t="dataTable" ref="AQ73:AQ102" dt2D="0" dtr="0" r1="W42" ca="1"/>
         <v>0.97608040491649806</v>
       </c>
       <c r="AR73" s="2">
@@ -37664,18 +37606,18 @@
       </c>
     </row>
     <row r="104" spans="26:46" x14ac:dyDescent="0.2">
-      <c r="Z104" s="33" t="s">
+      <c r="Z104" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="AA104" s="33"/>
-      <c r="AB104" s="33"/>
-      <c r="AC104" s="33"/>
-      <c r="AD104" s="33"/>
-      <c r="AE104" s="33"/>
-      <c r="AF104" s="33"/>
-      <c r="AG104" s="33"/>
-      <c r="AH104" s="33"/>
-      <c r="AI104" s="33"/>
+      <c r="AA104" s="43"/>
+      <c r="AB104" s="43"/>
+      <c r="AC104" s="43"/>
+      <c r="AD104" s="43"/>
+      <c r="AE104" s="43"/>
+      <c r="AF104" s="43"/>
+      <c r="AG104" s="43"/>
+      <c r="AH104" s="43"/>
+      <c r="AI104" s="43"/>
     </row>
     <row r="105" spans="26:46" x14ac:dyDescent="0.2">
       <c r="Z105" s="8" t="s">
@@ -37749,7 +37691,7 @@
         <v>2.8274333882308138</v>
       </c>
       <c r="AD107" s="2">
-        <f t="dataTable" ref="AD107:AD136" dt2D="0" dtr="0" r1="S61" ca="1"/>
+        <f t="dataTable" ref="AD107:AD136" dt2D="0" dtr="0" r1="S61"/>
         <v>0.23386125212353859</v>
       </c>
       <c r="AE107" s="2">
@@ -37757,7 +37699,7 @@
         <v>1.4294246573833558</v>
       </c>
       <c r="AF107" s="2">
-        <f t="dataTable" ref="AF107:AF136" dt2D="0" dtr="0" r1="S61"/>
+        <f t="dataTable" ref="AF107:AF136" dt2D="0" dtr="0" r1="S61" ca="1"/>
         <v>0.97358925215015468</v>
       </c>
       <c r="AG107" s="2">
@@ -38877,39 +38819,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="Z2:AI2"/>
-    <mergeCell ref="Z104:AI104"/>
-    <mergeCell ref="AK2:AT2"/>
-    <mergeCell ref="Z36:AI36"/>
-    <mergeCell ref="AK36:AT36"/>
-    <mergeCell ref="Z70:AI70"/>
-    <mergeCell ref="AK70:AT70"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="V22:X22"/>
-    <mergeCell ref="BC3:BE3"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="AZ3:BB3"/>
-    <mergeCell ref="R41:T41"/>
-    <mergeCell ref="V41:X41"/>
-    <mergeCell ref="R60:T60"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="N12:P12"/>
     <mergeCell ref="J21:L21"/>
     <mergeCell ref="N21:P21"/>
     <mergeCell ref="J30:L30"/>
@@ -38923,6 +38832,39 @@
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="N12:P12"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="BC3:BE3"/>
+    <mergeCell ref="AW3:AY3"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="R41:T41"/>
+    <mergeCell ref="V41:X41"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="Z2:AI2"/>
+    <mergeCell ref="Z104:AI104"/>
+    <mergeCell ref="AK2:AT2"/>
+    <mergeCell ref="Z36:AI36"/>
+    <mergeCell ref="AK36:AT36"/>
+    <mergeCell ref="Z70:AI70"/>
+    <mergeCell ref="AK70:AT70"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="V22:X22"/>
+    <mergeCell ref="R60:T60"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38994,97 +38936,97 @@
       <c r="BL2" s="2"/>
     </row>
     <row r="3" spans="2:71" x14ac:dyDescent="0.2">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37" t="s">
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
       <c r="N3"/>
-      <c r="O3" s="37" t="s">
+      <c r="O3" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37" t="s">
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37" t="s">
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="AA3" s="37" t="s">
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="AA3" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37" t="s">
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37" t="s">
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AM3" s="37" t="s">
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="48"/>
+      <c r="AM3" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="AN3" s="37"/>
-      <c r="AO3" s="37"/>
-      <c r="AP3" s="37" t="s">
+      <c r="AN3" s="48"/>
+      <c r="AO3" s="48"/>
+      <c r="AP3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="AQ3" s="37"/>
-      <c r="AR3" s="37"/>
-      <c r="AS3" s="37" t="s">
+      <c r="AQ3" s="48"/>
+      <c r="AR3" s="48"/>
+      <c r="AS3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="AT3" s="37"/>
-      <c r="AU3" s="37"/>
-      <c r="AY3" s="37" t="s">
+      <c r="AT3" s="48"/>
+      <c r="AU3" s="48"/>
+      <c r="AY3" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="AZ3" s="37"/>
-      <c r="BA3" s="37"/>
-      <c r="BB3" s="37" t="s">
+      <c r="AZ3" s="48"/>
+      <c r="BA3" s="48"/>
+      <c r="BB3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="BC3" s="37"/>
-      <c r="BD3" s="37"/>
-      <c r="BE3" s="37" t="s">
+      <c r="BC3" s="48"/>
+      <c r="BD3" s="48"/>
+      <c r="BE3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="BF3" s="37"/>
-      <c r="BG3" s="37"/>
-      <c r="BK3" s="37" t="s">
+      <c r="BF3" s="48"/>
+      <c r="BG3" s="48"/>
+      <c r="BK3" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="BL3" s="37"/>
-      <c r="BM3" s="37"/>
-      <c r="BN3" s="37" t="s">
+      <c r="BL3" s="48"/>
+      <c r="BM3" s="48"/>
+      <c r="BN3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="BO3" s="37"/>
-      <c r="BP3" s="37"/>
-      <c r="BQ3" s="37" t="s">
+      <c r="BO3" s="48"/>
+      <c r="BP3" s="48"/>
+      <c r="BQ3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="BR3" s="37"/>
-      <c r="BS3" s="37"/>
+      <c r="BR3" s="48"/>
+      <c r="BS3" s="48"/>
     </row>
     <row r="4" spans="2:71" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
@@ -45829,6 +45771,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="AA3:AC3"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="AG3:AI3"/>
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="BN3:BP3"/>
     <mergeCell ref="BQ3:BS3"/>
     <mergeCell ref="AS3:AU3"/>
@@ -45836,17 +45789,6 @@
     <mergeCell ref="BB3:BD3"/>
     <mergeCell ref="BE3:BG3"/>
     <mergeCell ref="BK3:BM3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="AG3:AI3"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45859,7 +45801,7 @@
   <dimension ref="B2:L69"/>
   <sheetViews>
     <sheetView zoomScale="106" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45876,98 +45818,98 @@
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="40" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="43">
+      <c r="C4" s="36">
         <v>0</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="2">
         <v>0.13220000000000001</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="36">
         <v>5.8400000000000001E-2</v>
       </c>
       <c r="F4" s="20">
         <v>0</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="38" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="43">
+      <c r="C5" s="36">
         <v>0.05</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="2">
         <v>0.128</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="36">
         <v>5.8200000000000002E-2</v>
       </c>
       <c r="F5" s="20">
         <v>0.11</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="39" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="43">
+      <c r="C6" s="36">
         <v>0.1</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="2">
         <v>0.12239999999999999</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="36">
         <v>5.7799999999999997E-2</v>
       </c>
       <c r="F6" s="20">
         <v>0.21199999999999999</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="39" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="43">
+      <c r="C7" s="36">
         <v>0.15</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="2">
         <v>0.11650000000000001</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="36">
         <v>5.7200000000000001E-2</v>
       </c>
       <c r="F7" s="20">
         <v>0.30599999999999999</v>
       </c>
-      <c r="H7" s="47" t="s">
+      <c r="H7" s="39" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="43">
+      <c r="C8" s="36">
         <v>0.2</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="2">
         <v>0.1101</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="36">
         <v>5.6399999999999999E-2</v>
       </c>
       <c r="F8" s="20">
@@ -45975,13 +45917,13 @@
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="43">
+      <c r="C9" s="36">
         <v>0.25</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="2">
         <v>0.1036</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="36">
         <v>5.5500000000000001E-2</v>
       </c>
       <c r="F9" s="20">
@@ -45989,13 +45931,13 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="43">
+      <c r="C10" s="36">
         <v>0.3</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="2">
         <v>9.6799999999999997E-2</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="36">
         <v>5.4300000000000001E-2</v>
       </c>
       <c r="F10" s="20">
@@ -46003,13 +45945,13 @@
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="43">
+      <c r="C11" s="36">
         <v>0.35</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="2">
         <v>8.9899999999999994E-2</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="36">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F11" s="20">
@@ -46017,13 +45959,13 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="43">
+      <c r="C12" s="36">
         <v>0.4</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="2">
         <v>8.2600000000000007E-2</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="36">
         <v>5.1400000000000001E-2</v>
       </c>
       <c r="F12" s="20">
@@ -46031,13 +45973,13 @@
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="43">
+      <c r="C13" s="36">
         <v>0.45</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="2">
         <v>7.5200000000000003E-2</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="36">
         <v>4.9200000000000001E-2</v>
       </c>
       <c r="F13" s="20">
@@ -46045,13 +45987,13 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="43">
+      <c r="C14" s="36">
         <v>0.5</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="2">
         <v>6.7400000000000002E-2</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="36">
         <v>4.6100000000000002E-2</v>
       </c>
       <c r="F14" s="20">
@@ -46059,13 +46001,13 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="43">
+      <c r="C15" s="36">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="2">
         <v>5.8700000000000002E-2</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="36">
         <v>4.19E-2</v>
       </c>
       <c r="F15" s="20">
@@ -46073,13 +46015,13 @@
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C16" s="43">
+      <c r="C16" s="36">
         <v>0.6</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="2">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="36">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F16" s="20">
@@ -46087,13 +46029,13 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C17" s="43">
+      <c r="C17" s="36">
         <v>0.65</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="2">
         <v>3.9100000000000003E-2</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="36">
         <v>3.1399999999999997E-2</v>
       </c>
       <c r="F17" s="20">
@@ -46101,13 +46043,13 @@
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C18" s="43">
+      <c r="C18" s="36">
         <v>0.7</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="2">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="36">
         <v>2.52E-2</v>
       </c>
       <c r="F18" s="20">
@@ -46115,13 +46057,13 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C19" s="43">
+      <c r="C19" s="36">
         <v>0.75</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="2">
         <v>1.83E-2</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="36">
         <v>1.8200000000000001E-2</v>
       </c>
       <c r="F19" s="20">
@@ -46129,13 +46071,13 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C20" s="44">
+      <c r="C20" s="37">
         <v>0.8</v>
       </c>
       <c r="D20" s="21">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E20" s="44">
+      <c r="E20" s="37">
         <v>1.06E-2</v>
       </c>
       <c r="F20" s="22">
@@ -46152,947 +46094,947 @@
       <c r="F22" s="49"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="41" t="s">
+      <c r="F23" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="43" cm="1">
+      <c r="B24" s="36" cm="1">
         <f t="array" ref="B24:B69">_xlfn.SEQUENCE(46,1,0,1)</f>
         <v>0</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="36">
         <f>B24*60/(1100*3.054)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="50">
+      <c r="D24" s="41">
         <v>0.13756114149530227</v>
       </c>
-      <c r="E24" s="51">
+      <c r="E24" s="42">
         <v>5.2588148987480245E-2</v>
       </c>
       <c r="F24" s="18">
         <v>0</v>
       </c>
-      <c r="H24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="H24" s="2"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="43">
+      <c r="B25" s="36">
         <v>1</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="36">
         <f>B25*60/(1100*3.054)</f>
         <v>1.7860332202178964E-2</v>
       </c>
       <c r="D25" s="19">
         <v>0.13900706290509893</v>
       </c>
-      <c r="E25" s="43">
+      <c r="E25" s="36">
         <v>5.4082694263797942E-2</v>
       </c>
       <c r="F25" s="20">
         <v>4.5905855019433478E-2</v>
       </c>
-      <c r="H25" s="38"/>
-      <c r="J25" s="38"/>
+      <c r="H25" s="2"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="43">
+      <c r="B26" s="36">
         <v>2</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="36">
         <f t="shared" ref="C26:C38" si="0">B26*60/(1100*3.054)</f>
         <v>3.5720664404357928E-2</v>
       </c>
       <c r="D26" s="19">
         <v>0.13687327609543906</v>
       </c>
-      <c r="E26" s="43">
+      <c r="E26" s="36">
         <v>5.4248917972665969E-2</v>
       </c>
       <c r="F26" s="20">
         <v>9.0125380266454239E-2</v>
       </c>
-      <c r="H26" s="38"/>
-      <c r="J26" s="38"/>
+      <c r="H26" s="2"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="43">
+      <c r="B27" s="36">
         <v>3</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="36">
         <f t="shared" si="0"/>
         <v>5.3580996606536889E-2</v>
       </c>
       <c r="D27" s="19">
         <v>0.13468643485481518</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="36">
         <v>5.4388139009096559E-2</v>
       </c>
       <c r="F27" s="20">
         <v>0.13268763264165745</v>
       </c>
-      <c r="H27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="H27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="43">
+      <c r="B28" s="36">
         <v>4</v>
       </c>
-      <c r="C28" s="43">
+      <c r="C28" s="36">
         <f t="shared" si="0"/>
         <v>7.1441328808715857E-2</v>
       </c>
       <c r="D28" s="19">
-        <v>0.13244612392823049</v>
-      </c>
-      <c r="E28" s="43">
+        <v>0.13244612392822999</v>
+      </c>
+      <c r="E28" s="36">
         <v>5.4498255617636729E-2</v>
       </c>
       <c r="F28" s="20">
         <v>0.17362256794756029</v>
       </c>
-      <c r="H28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="H28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="43">
+      <c r="B29" s="36">
         <v>5</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="36">
         <f t="shared" si="0"/>
         <v>8.9301661010894817E-2</v>
       </c>
       <c r="D29" s="19">
         <v>0.130152000348078</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="36">
         <v>5.4577101702351034E-2</v>
       </c>
       <c r="F29" s="20">
         <v>0.21296092046736914</v>
       </c>
-      <c r="H29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="H29" s="2"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B30" s="43">
+      <c r="B30" s="36">
         <v>6</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="36">
         <f t="shared" si="0"/>
         <v>0.10716199321307378</v>
       </c>
       <c r="D30" s="19">
         <v>0.12780379143048623</v>
       </c>
-      <c r="E30" s="43">
+      <c r="E30" s="36">
         <v>5.4622449587135073E-2</v>
       </c>
       <c r="F30" s="20">
         <v>0.25073406874642507</v>
       </c>
-      <c r="H30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="H30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="43">
+      <c r="B31" s="36">
         <v>7</v>
       </c>
-      <c r="C31" s="43">
+      <c r="C31" s="36">
         <f t="shared" si="0"/>
         <v>0.12502232541525274</v>
       </c>
       <c r="D31" s="19">
         <v>0.12540129088350571</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="36">
         <v>5.4632014768505488E-2</v>
       </c>
       <c r="F31" s="20">
         <v>0.28697387535062174</v>
       </c>
-      <c r="H31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="H31" s="2"/>
+      <c r="J31" s="2"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="43">
+      <c r="B32" s="36">
         <v>8</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="36">
         <f t="shared" si="0"/>
         <v>0.14288265761743171</v>
       </c>
       <c r="D32" s="19">
         <v>0.12294437025873374</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="36">
         <v>5.4603462101377245E-2</v>
       </c>
       <c r="F32" s="20">
         <v>0.32171253773350622</v>
       </c>
-      <c r="H32" s="38"/>
-      <c r="J32" s="38"/>
+      <c r="H32" s="2"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="43">
+      <c r="B33" s="36">
         <v>9</v>
       </c>
-      <c r="C33" s="43">
+      <c r="C33" s="36">
         <f t="shared" si="0"/>
         <v>0.16074298981961066</v>
       </c>
       <c r="D33" s="19">
         <v>0.12043296699527706</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="36">
         <v>5.4534410555322911E-2</v>
       </c>
       <c r="F33" s="20">
         <v>0.35498238617668137</v>
       </c>
-      <c r="H33" s="38"/>
-      <c r="J33" s="38"/>
+      <c r="H33" s="2"/>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="43">
+      <c r="B34" s="36">
         <v>10</v>
       </c>
-      <c r="C34" s="43">
+      <c r="C34" s="36">
         <f t="shared" si="0"/>
         <v>0.17860332202178963</v>
       </c>
       <c r="D34" s="19">
         <v>0.11786709903466028</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="36">
         <v>5.4422440954226992E-2</v>
       </c>
       <c r="F34" s="20">
         <v>0.38681571564140826</v>
       </c>
-      <c r="H34" s="38"/>
-      <c r="J34" s="38"/>
+      <c r="H34" s="2"/>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B35" s="43">
+      <c r="B35" s="36">
         <v>11</v>
       </c>
-      <c r="C35" s="43">
+      <c r="C35" s="36">
         <f t="shared" si="0"/>
         <v>0.19646365422396858</v>
       </c>
       <c r="D35" s="19">
         <v>0.11524684278473754</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="36">
         <v>5.4265099849561585E-2</v>
       </c>
       <c r="F35" s="20">
         <v>0.4172445261141019</v>
       </c>
-      <c r="H35" s="38"/>
-      <c r="J35" s="38"/>
+      <c r="H35" s="2"/>
+      <c r="J35" s="2"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="43">
+      <c r="B36" s="36">
         <v>12</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C36" s="36">
         <f t="shared" si="0"/>
         <v>0.21432398642614756</v>
       </c>
       <c r="D36" s="19">
         <v>0.11257235615034641</v>
       </c>
-      <c r="E36" s="43">
+      <c r="E36" s="36">
         <v>5.4059909541711047E-2</v>
       </c>
       <c r="F36" s="20">
         <v>0.44630034226954524</v>
       </c>
-      <c r="H36" s="38"/>
-      <c r="J36" s="38"/>
+      <c r="H36" s="2"/>
+      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B37" s="43">
+      <c r="B37" s="36">
         <v>13</v>
       </c>
-      <c r="C37" s="43">
+      <c r="C37" s="36">
         <f t="shared" si="0"/>
         <v>0.2321843186283265</v>
       </c>
       <c r="D37" s="19">
         <v>0.10984385704477058</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="36">
         <v>5.3804372180135722E-2</v>
       </c>
       <c r="F37" s="20">
         <v>0.4740139150413375</v>
       </c>
-      <c r="H37" s="38"/>
-      <c r="J37" s="38"/>
+      <c r="H37" s="2"/>
+      <c r="J37" s="2"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="43">
+      <c r="B38" s="36">
         <v>14</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="36">
         <f t="shared" si="0"/>
         <v>0.25004465083050548</v>
       </c>
       <c r="D38" s="19">
         <v>0.10706163067370951</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="36">
         <v>5.3495978015493717E-2</v>
       </c>
       <c r="F38" s="20">
         <v>0.5004149667363581</v>
       </c>
-      <c r="H38" s="38"/>
-      <c r="J38" s="38"/>
+      <c r="H38" s="2"/>
+      <c r="J38" s="2"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" s="43">
+      <c r="B39" s="36">
         <v>15</v>
       </c>
-      <c r="C39" s="43">
+      <c r="C39" s="36">
         <f>B39*60/(1100*3.054)</f>
         <v>0.26790498303268445</v>
       </c>
       <c r="D39" s="19">
         <v>0.10422602209693513</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="36">
         <v>5.3132211963645572E-2</v>
       </c>
       <c r="F39" s="20">
         <v>0.52553186945329911</v>
       </c>
-      <c r="H39" s="38"/>
-      <c r="J39" s="38"/>
+      <c r="H39" s="2"/>
+      <c r="J39" s="2"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="43">
+      <c r="B40" s="36">
         <v>16</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C40" s="36">
         <f>B40*60/(1100*3.054)</f>
         <v>0.28576531523486343</v>
       </c>
       <c r="D40" s="19">
         <v>0.10133743682024815</v>
       </c>
-      <c r="E40" s="43">
+      <c r="E40" s="36">
         <v>5.2710561000284817E-2</v>
       </c>
       <c r="F40" s="20">
         <v>0.54939131795381169</v>
       </c>
-      <c r="H40" s="38"/>
-      <c r="J40" s="38"/>
+      <c r="H40" s="2"/>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="43">
+      <c r="B41" s="36">
         <v>17</v>
       </c>
-      <c r="C41" s="43">
+      <c r="C41" s="36">
         <f t="shared" ref="C41:C69" si="1">B41*60/(1100*3.054)</f>
         <v>0.30362564743704235</v>
       </c>
       <c r="D41" s="19">
         <v>9.8396332682932228E-2</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="36">
         <v>5.2228520118700737E-2</v>
       </c>
       <c r="F41" s="20">
         <v>0.57201793480625063</v>
       </c>
-      <c r="H41" s="38"/>
-      <c r="J41" s="38"/>
+      <c r="H41" s="2"/>
+      <c r="J41" s="2"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="19">
         <v>18</v>
       </c>
-      <c r="C42" s="43">
+      <c r="C42" s="36">
         <f t="shared" si="1"/>
         <v>0.32148597963922132</v>
       </c>
       <c r="D42" s="19">
         <v>9.5403220360501251E-2</v>
       </c>
-      <c r="E42" s="43">
+      <c r="E42" s="36">
         <v>5.1683599726241938E-2</v>
       </c>
       <c r="F42" s="20">
         <v>0.59343385369419988</v>
       </c>
-      <c r="H42" s="38"/>
-      <c r="J42" s="38"/>
+      <c r="H42" s="2"/>
+      <c r="J42" s="2"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B43" s="19">
         <v>19</v>
       </c>
-      <c r="C43" s="43">
+      <c r="C43" s="36">
         <f t="shared" si="1"/>
         <v>0.33934631184140029</v>
       </c>
       <c r="D43" s="19">
         <v>9.2358650601593553E-2</v>
       </c>
-      <c r="E43" s="43">
+      <c r="E43" s="36">
         <v>5.1073330068599425E-2</v>
       </c>
       <c r="F43" s="20">
         <v>0.61365819315487558</v>
       </c>
-      <c r="H43" s="38"/>
-      <c r="J43" s="38"/>
+      <c r="H43" s="2"/>
+      <c r="J43" s="2"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B44" s="19">
         <v>20</v>
       </c>
-      <c r="C44" s="43">
+      <c r="C44" s="36">
         <f t="shared" si="1"/>
         <v>0.35720664404357927</v>
       </c>
       <c r="D44" s="19">
         <v>8.9263222154719948E-2</v>
       </c>
-      <c r="E44" s="43">
+      <c r="E44" s="36">
         <v>5.0395270131194138E-2</v>
       </c>
       <c r="F44" s="20">
         <v>0.63270652065951039</v>
       </c>
-      <c r="H44" s="38"/>
-      <c r="J44" s="38"/>
+      <c r="H44" s="2"/>
+      <c r="J44" s="2"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B45" s="19">
         <v>21</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C45" s="36">
         <f t="shared" si="1"/>
         <v>0.37506697624575819</v>
       </c>
       <c r="D45" s="19">
         <v>8.611756323739439E-2</v>
       </c>
-      <c r="E45" s="43">
+      <c r="E45" s="36">
         <v>4.9647009681194371E-2</v>
       </c>
       <c r="F45" s="20">
         <v>0.65059012118784543</v>
       </c>
-      <c r="H45" s="38"/>
-      <c r="J45" s="38"/>
+      <c r="H45" s="2"/>
+      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B46" s="19">
         <v>22</v>
       </c>
-      <c r="C46" s="43">
+      <c r="C46" s="36">
         <f t="shared" si="1"/>
         <v>0.39292730844793716</v>
       </c>
       <c r="D46" s="19">
         <v>8.2922336819380466E-2</v>
       </c>
-      <c r="E46" s="43">
+      <c r="E46" s="36">
         <v>4.8826176719182254E-2</v>
       </c>
       <c r="F46" s="20">
         <v>0.66731521503406666</v>
       </c>
-      <c r="H46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="H46" s="2"/>
+      <c r="J46" s="2"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B47" s="19">
         <v>23</v>
       </c>
-      <c r="C47" s="43">
+      <c r="C47" s="36">
         <f t="shared" si="1"/>
         <v>0.41078764065011614</v>
       </c>
       <c r="D47" s="19">
         <v>7.9678231508325606E-2</v>
       </c>
-      <c r="E47" s="43">
+      <c r="E47" s="36">
         <v>4.7930441166935414E-2</v>
       </c>
       <c r="F47" s="20">
         <v>0.68288194173889694</v>
       </c>
-      <c r="H47" s="38"/>
-      <c r="J47" s="38"/>
+      <c r="H47" s="2"/>
+      <c r="J47" s="2"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B48" s="19">
         <v>24</v>
       </c>
-      <c r="C48" s="43">
+      <c r="C48" s="36">
         <f t="shared" si="1"/>
         <v>0.42864797285229511</v>
       </c>
       <c r="D48" s="19">
         <v>7.638595659731566E-2</v>
       </c>
-      <c r="E48" s="43">
+      <c r="E48" s="36">
         <v>4.6957518943194825E-2</v>
       </c>
       <c r="F48" s="20">
         <v>0.69728312284624838</v>
       </c>
-      <c r="H48" s="38"/>
-      <c r="J48" s="38"/>
+      <c r="H48" s="2"/>
+      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B49" s="19">
         <v>25</v>
       </c>
-      <c r="C49" s="43">
+      <c r="C49" s="36">
         <f t="shared" si="1"/>
         <v>0.44650830505447409</v>
       </c>
       <c r="D49" s="19">
         <v>7.3046238743475406E-2</v>
       </c>
-      <c r="E49" s="43">
+      <c r="E49" s="36">
         <v>4.5905175709907271E-2</v>
       </c>
       <c r="F49" s="20">
         <v>0.71050272104534196</v>
       </c>
-      <c r="H49" s="38"/>
-      <c r="J49" s="38"/>
+      <c r="H49" s="2"/>
+      <c r="J49" s="2"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="19">
         <v>26</v>
       </c>
-      <c r="C50" s="43">
+      <c r="C50" s="36">
         <f t="shared" si="1"/>
         <v>0.46436863725665301</v>
       </c>
       <c r="D50" s="19">
         <v>6.9659815418716103E-2</v>
       </c>
-      <c r="E50" s="43">
+      <c r="E50" s="36">
         <v>4.477122964425307E-2</v>
       </c>
       <c r="F50" s="20">
         <v>0.72251385129627366</v>
       </c>
-      <c r="H50" s="38"/>
-      <c r="J50" s="38"/>
+      <c r="H50" s="2"/>
+      <c r="J50" s="2"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="19">
         <v>27</v>
       </c>
-      <c r="C51" s="43">
+      <c r="C51" s="36">
         <f t="shared" si="1"/>
         <v>0.48222896945883198</v>
       </c>
       <c r="D51" s="19">
         <v>6.6227430577614307E-2</v>
       </c>
-      <c r="E51" s="43">
+      <c r="E51" s="36">
         <v>4.3553553662657195E-2</v>
       </c>
       <c r="F51" s="20">
         <v>0.73327622918475832</v>
       </c>
-      <c r="H51" s="38"/>
-      <c r="J51" s="38"/>
+      <c r="H51" s="2"/>
+      <c r="J51" s="2"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="19">
         <v>28</v>
       </c>
-      <c r="C52" s="43">
+      <c r="C52" s="36">
         <f t="shared" si="1"/>
         <v>0.50008930166101095</v>
       </c>
       <c r="D52" s="19">
         <v>6.2749833362113094E-2</v>
       </c>
-      <c r="E52" s="43">
+      <c r="E52" s="36">
         <v>4.2250078583909931E-2</v>
       </c>
       <c r="F52" s="20">
         <v>0.74273282789477613</v>
       </c>
-      <c r="H52" s="38"/>
-      <c r="J52" s="38"/>
+      <c r="H52" s="2"/>
+      <c r="J52" s="2"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" s="19">
         <v>29</v>
       </c>
-      <c r="C53" s="43">
+      <c r="C53" s="36">
         <f t="shared" si="1"/>
         <v>0.51794963386318993</v>
       </c>
       <c r="D53" s="19">
         <v>5.9227772381406377E-2</v>
       </c>
-      <c r="E53" s="43">
+      <c r="E53" s="36">
         <v>4.0858794452282646E-2</v>
       </c>
       <c r="F53" s="20">
         <v>0.750805387939388</v>
       </c>
-      <c r="H53" s="38"/>
-      <c r="J53" s="38"/>
+      <c r="H53" s="2"/>
+      <c r="J53" s="2"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" s="19">
         <v>30</v>
       </c>
-      <c r="C54" s="43">
+      <c r="C54" s="36">
         <f t="shared" si="1"/>
         <v>0.5358099660653689</v>
       </c>
       <c r="D54" s="19">
         <v>5.5661987509543508E-2</v>
       </c>
-      <c r="E54" s="43">
+      <c r="E54" s="36">
         <v>3.937774944449788E-2</v>
       </c>
       <c r="F54" s="20">
         <v>0.75738832359264596</v>
       </c>
-      <c r="H54" s="38"/>
-      <c r="J54" s="38"/>
+      <c r="H54" s="2"/>
+      <c r="J54" s="2"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B55" s="19">
         <v>31</v>
       </c>
-      <c r="C55" s="43">
+      <c r="C55" s="36">
         <f t="shared" si="1"/>
         <v>0.55367029826754788</v>
       </c>
       <c r="D55" s="19">
         <v>5.2053213750376616E-2</v>
       </c>
-      <c r="E55" s="43">
+      <c r="E55" s="36">
         <v>3.7805053446073308E-2</v>
       </c>
       <c r="F55" s="20">
         <v>0.76234036870403954</v>
       </c>
-      <c r="H55" s="38"/>
-      <c r="J55" s="38"/>
+      <c r="H55" s="2"/>
+      <c r="J55" s="2"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56" s="19">
         <v>32</v>
       </c>
-      <c r="C56" s="43">
+      <c r="C56" s="36">
         <f t="shared" si="1"/>
         <v>0.57153063046972685</v>
       </c>
       <c r="D56" s="19">
         <v>4.8402174324246629E-2</v>
       </c>
-      <c r="E56" s="43">
+      <c r="E56" s="36">
         <v>3.6138876930226757E-2</v>
       </c>
       <c r="F56" s="20">
         <v>0.76547274175265079</v>
       </c>
-      <c r="H56" s="38"/>
-      <c r="J56" s="38"/>
+      <c r="H56" s="2"/>
+      <c r="J56" s="2"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" s="19">
         <v>33</v>
       </c>
-      <c r="C57" s="43">
+      <c r="C57" s="36">
         <f t="shared" si="1"/>
         <v>0.58939096267190572</v>
       </c>
       <c r="D57" s="19">
         <v>4.4709578491025227E-2</v>
       </c>
-      <c r="E57" s="43">
+      <c r="E57" s="36">
         <v>3.4377451150045792E-2</v>
       </c>
       <c r="F57" s="20">
         <v>0.76653214900853361</v>
       </c>
-      <c r="H57" s="38"/>
-      <c r="J57" s="38"/>
+      <c r="H57" s="2"/>
+      <c r="J57" s="2"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B58" s="19">
         <v>34</v>
       </c>
-      <c r="C58" s="43">
+      <c r="C58" s="36">
         <f t="shared" si="1"/>
         <v>0.60725129487408469</v>
       </c>
       <c r="D58" s="19">
         <v>4.1543323116758443E-2</v>
       </c>
-      <c r="E58" s="43">
+      <c r="E58" s="36">
         <v>3.3208413976648005E-2</v>
       </c>
       <c r="F58" s="20">
         <v>0.75966400484418584</v>
       </c>
-      <c r="H58" s="38"/>
-      <c r="J58" s="38"/>
+      <c r="H58" s="2"/>
+      <c r="J58" s="2"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B59" s="19">
         <v>35</v>
       </c>
-      <c r="C59" s="43">
+      <c r="C59" s="36">
         <f t="shared" si="1"/>
         <v>0.62511162707626367</v>
       </c>
       <c r="D59" s="19">
         <v>3.7971951154892644E-2</v>
       </c>
-      <c r="E59" s="43">
+      <c r="E59" s="36">
         <v>3.1260643752866954E-2</v>
       </c>
       <c r="F59" s="20">
         <v>0.75931603831793859</v>
       </c>
-      <c r="H59" s="38"/>
-      <c r="J59" s="38"/>
+      <c r="H59" s="2"/>
+      <c r="J59" s="2"/>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B60" s="19">
         <v>36</v>
       </c>
-      <c r="C60" s="43">
+      <c r="C60" s="36">
         <f t="shared" si="1"/>
         <v>0.64297195927844264</v>
       </c>
       <c r="D60" s="19">
         <v>3.4366650775569448E-2</v>
       </c>
-      <c r="E60" s="43">
+      <c r="E60" s="36">
         <v>2.9215999168895716E-2</v>
       </c>
       <c r="F60" s="20">
         <v>0.75632507569793639</v>
       </c>
-      <c r="H60" s="38"/>
-      <c r="J60" s="38"/>
+      <c r="H60" s="2"/>
+      <c r="J60" s="2"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="19">
         <v>37</v>
       </c>
-      <c r="C61" s="43">
+      <c r="C61" s="36">
         <f t="shared" si="1"/>
         <v>0.66083229148062161</v>
       </c>
       <c r="D61" s="19">
         <v>3.0728073222855617E-2</v>
       </c>
-      <c r="E61" s="43">
+      <c r="E61" s="36">
         <v>2.7073060859561449E-2</v>
       </c>
       <c r="F61" s="20">
         <v>0.7500482913985862</v>
       </c>
-      <c r="H61" s="38"/>
-      <c r="J61" s="38"/>
+      <c r="H61" s="2"/>
+      <c r="J61" s="2"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B62" s="19">
         <v>38</v>
       </c>
-      <c r="C62" s="43">
+      <c r="C62" s="36">
         <f t="shared" si="1"/>
         <v>0.67869262368280059</v>
       </c>
       <c r="D62" s="19">
         <v>2.7056837308200583E-2</v>
       </c>
-      <c r="E62" s="43">
+      <c r="E62" s="36">
         <v>2.4830454913392794E-2</v>
       </c>
       <c r="F62" s="20">
         <v>0.73954649503246694</v>
       </c>
-      <c r="H62" s="38"/>
-      <c r="J62" s="38"/>
+      <c r="H62" s="2"/>
+      <c r="J62" s="2"/>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B63" s="19">
         <v>39</v>
       </c>
-      <c r="C63" s="43">
+      <c r="C63" s="36">
         <f t="shared" si="1"/>
         <v>0.69655295588497956</v>
       </c>
       <c r="D63" s="19">
         <v>2.3353540249377965E-2</v>
       </c>
-      <c r="E63" s="43">
+      <c r="E63" s="36">
         <v>2.24868576646267E-2</v>
       </c>
       <c r="F63" s="20">
         <v>0.72339931766776311</v>
       </c>
-      <c r="H63" s="38"/>
-      <c r="J63" s="38"/>
+      <c r="H63" s="2"/>
+      <c r="J63" s="2"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B64" s="19">
         <v>40</v>
       </c>
-      <c r="C64" s="43">
+      <c r="C64" s="36">
         <f t="shared" si="1"/>
         <v>0.71441328808715854</v>
       </c>
       <c r="D64" s="19">
         <v>1.9618751498962167E-2</v>
       </c>
-      <c r="E64" s="43">
+      <c r="E64" s="36">
         <v>2.0040991672569414E-2</v>
       </c>
       <c r="F64" s="20">
         <v>0.69936143857204069</v>
       </c>
-      <c r="H64" s="38"/>
-      <c r="J64" s="38"/>
+      <c r="H64" s="2"/>
+      <c r="J64" s="2"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B65" s="19">
         <v>41</v>
       </c>
-      <c r="C65" s="43">
+      <c r="C65" s="36">
         <f t="shared" si="1"/>
         <v>0.73227362028933751</v>
       </c>
       <c r="D65" s="19">
         <v>1.5853013965171921E-2</v>
       </c>
-      <c r="E65" s="43">
+      <c r="E65" s="36">
         <v>1.7491624618448474E-2</v>
       </c>
       <c r="F65" s="20">
         <v>0.66367442601815763</v>
       </c>
-      <c r="H65" s="38"/>
-      <c r="J65" s="38"/>
+      <c r="H65" s="2"/>
+      <c r="J65" s="2"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B66" s="19">
         <v>42</v>
       </c>
-      <c r="C66" s="43">
+      <c r="C66" s="36">
         <f t="shared" si="1"/>
         <v>0.75013395249151638</v>
       </c>
       <c r="D66" s="19">
         <v>1.2056846041127757E-2</v>
       </c>
-      <c r="E66" s="43">
+      <c r="E66" s="36">
         <v>1.4837569799811086E-2</v>
       </c>
       <c r="F66" s="20">
         <v>0.60955060009409423</v>
       </c>
-      <c r="H66" s="38"/>
-      <c r="J66" s="38"/>
+      <c r="H66" s="2"/>
+      <c r="J66" s="2"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B67" s="19">
         <v>43</v>
       </c>
-      <c r="C67" s="43">
+      <c r="C67" s="36">
         <f t="shared" si="1"/>
         <v>0.76799428469369535</v>
       </c>
       <c r="D67" s="19">
         <v>9.478771566653544E-3</v>
       </c>
-      <c r="E67" s="43">
+      <c r="E67" s="36">
         <v>1.3969921951479934E-2</v>
       </c>
       <c r="F67" s="20">
         <v>0.52109399139025547</v>
       </c>
-      <c r="H67" s="38"/>
-      <c r="J67" s="38"/>
+      <c r="H67" s="2"/>
+      <c r="J67" s="2"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B68" s="19">
         <v>44</v>
       </c>
-      <c r="C68" s="43">
+      <c r="C68" s="36">
         <f t="shared" si="1"/>
         <v>0.78585461689587432</v>
       </c>
       <c r="D68" s="19">
         <v>5.9745670722236117E-3</v>
       </c>
-      <c r="E68" s="43">
+      <c r="E68" s="36">
         <v>1.113815586381486E-2</v>
       </c>
       <c r="F68" s="20">
         <v>0.42153666864317774</v>
       </c>
-      <c r="H68" s="38"/>
-      <c r="J68" s="38"/>
+      <c r="H68" s="2"/>
+      <c r="J68" s="2"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B69" s="39">
+      <c r="B69" s="32">
         <v>45</v>
       </c>
-      <c r="C69" s="44">
+      <c r="C69" s="37">
         <f t="shared" si="1"/>
         <v>0.8037149490980533</v>
       </c>
-      <c r="D69" s="39">
+      <c r="D69" s="32">
         <v>2.4488326488181986E-3</v>
       </c>
-      <c r="E69" s="44">
+      <c r="E69" s="37">
         <v>8.2051630940321672E-3</v>
       </c>
       <c r="F69" s="22">
         <v>0.2398688953698028</v>
       </c>
-      <c r="H69" s="38"/>
-      <c r="J69" s="38"/>
+      <c r="H69" s="2"/>
+      <c r="J69" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
added BEMT with grads in OpenMDAO
</commit_message>
<xml_diff>
--- a/sheets/BEMT.xlsx
+++ b/sheets/BEMT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50AF903-446A-AC48-963E-A1FACF966845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA46C16-88BA-6845-B3CD-91458BB8FE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{3818933C-C78F-A44D-BD0C-A20632FBDB3F}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="122">
   <si>
     <t>[case]</t>
   </si>
@@ -28136,7 +28136,7 @@
   <dimension ref="B2:BE136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="N21" sqref="N21:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29785,8 +29785,8 @@
         <v>100</v>
       </c>
       <c r="G15" s="2">
-        <f>SQRT(G10^3/(2*C41*PI()*(C8/2)^2))/1000</f>
-        <v>82.927947944833036</v>
+        <f>G10*(C3/2 + SQRT( (C3/2)^2 + (G10/(2*C41*PI()*G3^2))) )/1000</f>
+        <v>85.454746924080695</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>99</v>
@@ -29912,7 +29912,7 @@
       </c>
       <c r="G16" s="2">
         <f>G15/G12</f>
-        <v>0.76460484091480463</v>
+        <v>0.7879022066332545</v>
       </c>
       <c r="H16" s="3"/>
       <c r="J16" s="2" t="s">
@@ -38872,10 +38872,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF676D7-47B6-0F44-A1F9-CF984FF81BA6}">
-  <dimension ref="B2:BS117"/>
+  <dimension ref="B2:CE117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38893,7 +38893,7 @@
     <col min="61" max="61" width="3.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B2" s="14" t="s">
         <v>50</v>
       </c>
@@ -38934,8 +38934,15 @@
         <v>121</v>
       </c>
       <c r="BL2" s="2"/>
+      <c r="BV2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BX2" s="2"/>
     </row>
-    <row r="3" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:83" x14ac:dyDescent="0.2">
       <c r="C3" s="48" t="s">
         <v>60</v>
       </c>
@@ -39027,8 +39034,23 @@
       </c>
       <c r="BR3" s="48"/>
       <c r="BS3" s="48"/>
+      <c r="BW3" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="BX3" s="48"/>
+      <c r="BY3" s="48"/>
+      <c r="BZ3" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="CA3" s="48"/>
+      <c r="CB3" s="48"/>
+      <c r="CC3" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="CD3" s="48"/>
+      <c r="CE3" s="48"/>
     </row>
-    <row r="4" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:83" x14ac:dyDescent="0.2">
       <c r="C4" s="5" t="s">
         <v>63</v>
       </c>
@@ -39141,8 +39163,24 @@
       </c>
       <c r="BR4" s="2"/>
       <c r="BS4" s="2"/>
+      <c r="BV4" s="2"/>
+      <c r="BW4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX4" s="7"/>
+      <c r="BY4" s="7"/>
+      <c r="BZ4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="CA4" s="2"/>
+      <c r="CB4" s="2"/>
+      <c r="CC4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="CD4" s="2"/>
+      <c r="CE4" s="2"/>
     </row>
-    <row r="5" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
@@ -39223,8 +39261,18 @@
       <c r="BO5" s="10"/>
       <c r="BP5" s="10"/>
       <c r="BQ5" s="10"/>
+      <c r="BV5" t="s">
+        <v>52</v>
+      </c>
+      <c r="BW5" s="7"/>
+      <c r="BX5" s="7"/>
+      <c r="BY5" s="10"/>
+      <c r="BZ5" s="10"/>
+      <c r="CA5" s="10"/>
+      <c r="CB5" s="10"/>
+      <c r="CC5" s="10"/>
     </row>
-    <row r="6" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B6" s="14" t="s">
         <v>53</v>
       </c>
@@ -39305,8 +39353,18 @@
       <c r="BO6" s="10"/>
       <c r="BP6" s="10"/>
       <c r="BQ6" s="10"/>
+      <c r="BV6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BW6" s="7"/>
+      <c r="BX6" s="7"/>
+      <c r="BY6" s="10"/>
+      <c r="BZ6" s="10"/>
+      <c r="CA6" s="10"/>
+      <c r="CB6" s="10"/>
+      <c r="CC6" s="10"/>
     </row>
-    <row r="7" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:83" x14ac:dyDescent="0.2">
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
@@ -39320,7 +39378,7 @@
       <c r="BK7" s="2"/>
       <c r="BL7" s="2"/>
     </row>
-    <row r="8" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>47</v>
       </c>
@@ -39400,8 +39458,17 @@
       <c r="BL8" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="BV8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="BW8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="BX8" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="9" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>-180</v>
       </c>
@@ -39483,7 +39550,7 @@
         <v>7.9652736000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>-176.363636363636</v>
       </c>
@@ -39563,7 +39630,7 @@
         <v>8.2075064419237106E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>-172.72727272727201</v>
       </c>
@@ -39638,7 +39705,7 @@
         <v>9.8626242426573404E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>-169.09090909090901</v>
       </c>
@@ -39718,7 +39785,7 @@
         <v>0.14254193778124399</v>
       </c>
     </row>
-    <row r="13" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>-165.45454545454501</v>
       </c>
@@ -39798,7 +39865,7 @@
         <v>0.21516547684083201</v>
       </c>
     </row>
-    <row r="14" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>-161.81818181818099</v>
       </c>
@@ -39873,7 +39940,7 @@
         <v>0.28708838802095399</v>
       </c>
     </row>
-    <row r="15" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>-158.18181818181799</v>
       </c>
@@ -39953,7 +40020,7 @@
         <v>0.34429008436838299</v>
       </c>
     </row>
-    <row r="16" spans="2:71" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>-154.54545454545399</v>
       </c>
@@ -45770,7 +45837,7 @@
       <c r="I117" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="21">
     <mergeCell ref="U3:W3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="I3:K3"/>
@@ -45782,13 +45849,16 @@
     <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="AM3:AO3"/>
     <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="BN3:BP3"/>
-    <mergeCell ref="BQ3:BS3"/>
     <mergeCell ref="AS3:AU3"/>
     <mergeCell ref="AY3:BA3"/>
     <mergeCell ref="BB3:BD3"/>
     <mergeCell ref="BE3:BG3"/>
     <mergeCell ref="BK3:BM3"/>
+    <mergeCell ref="BW3:BY3"/>
+    <mergeCell ref="BZ3:CB3"/>
+    <mergeCell ref="CC3:CE3"/>
+    <mergeCell ref="BN3:BP3"/>
+    <mergeCell ref="BQ3:BS3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>